<commit_message>
Test Data , Test Util  changed
</commit_message>
<xml_diff>
--- a/PageObjectModelPractice2/src/main/java/com/crm/qa/testdata/Book1.xlsx
+++ b/PageObjectModelPractice2/src/main/java/com/crm/qa/testdata/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\NewEclipseWorkspace\PageObjectModelPractice2\src\main\java\com\crm\qa\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\git\POM2\PageObjectModelPractice2\src\main\java\com\crm\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -132,7 +132,7 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>bhargavjsh95@gmail.com</t>
+    <t>bhargavjsh91@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>